<commit_message>
Added all test cases for Header module
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/HeaderTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/HeaderTestData.xlsx
@@ -8,13 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="headerMainMenu" sheetId="1" r:id="rId1"/>
+    <sheet name="headerSubMenu" sheetId="2" r:id="rId2"/>
+    <sheet name="whereToBuy" sheetId="3" r:id="rId3"/>
+    <sheet name="language" sheetId="4" r:id="rId4"/>
+    <sheet name="search" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>testcase</t>
   </si>
@@ -31,13 +35,232 @@
     <t>Verify user is redirected to correct url after clicking on 'PRODUCTS' in the main horizontal menu</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>Products</t>
   </si>
   <si>
     <t>products</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Benadryl Difference' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Benadryl Difference</t>
+  </si>
+  <si>
+    <t>benadryl-difference</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Dosing Guide' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Dosing Guide</t>
+  </si>
+  <si>
+    <t>benadryl-dosing-guide</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Savings' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>save-on-benadryl</t>
+  </si>
+  <si>
+    <t>subMenu</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Adult under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>products/adult-oral</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Kid's under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <t>Kid's</t>
+  </si>
+  <si>
+    <t>products/kids</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Topical under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Topical</t>
+    </r>
+  </si>
+  <si>
+    <t>products/adult-topical</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>All Products</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Compare Benadryl under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Compare Benadryl</t>
+  </si>
+  <si>
+    <t>benadryl-difference/compare-allergy-relief-products</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Benadryl Uses" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Benadryl Difference</t>
+    </r>
+  </si>
+  <si>
+    <t>Benadryl Uses</t>
+  </si>
+  <si>
+    <t>benadryl-difference/uses-indications</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Our Ingredients" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Our Ingredients</t>
+  </si>
+  <si>
+    <t>benadryl-difference/ingredients-transparency</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "FAQ" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>faq</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Safety Information' under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Safety Information</t>
+  </si>
+  <si>
+    <t>safety</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "About Diphenhydramine" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>About Diphenhydramine</t>
+  </si>
+  <si>
+    <t>benadryl-difference/diphenhydramine-active-ingredient</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Allergies" under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Allergy &amp; Cold Guide</t>
+  </si>
+  <si>
+    <t>Allergies</t>
+  </si>
+  <si>
+    <t>allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Kid's Allergies' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Kid's Allergies</t>
+  </si>
+  <si>
+    <t>childrens-allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Itchy Skin' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Itchy Skin</t>
+  </si>
+  <si>
+    <t>itchy-skin</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Cold or Allergies?' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Cold or Allergies?</t>
+  </si>
+  <si>
+    <t>cold/cold-or-allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Where to buy' in the header</t>
+  </si>
+  <si>
+    <t>where-to-buy</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>Check that user can change the locale to 'Espanol'</t>
+  </si>
+  <si>
+    <t>Espanol</t>
+  </si>
+  <si>
+    <t>https://es.benadryl.com/</t>
+  </si>
+  <si>
+    <t>Check that user can change the locale to 'English'</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>https://www.benadryl.com/</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>Verify search functionality</t>
+  </si>
+  <si>
+    <t>Benadryl</t>
+  </si>
+  <si>
+    <t>search/site/Benadryl</t>
   </si>
 </sst>
 </file>
@@ -50,8 +273,16 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,6 +296,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -521,141 +758,151 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,13 +1222,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="95.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="20.7777777777778" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -998,21 +1249,490 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="106.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="21.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="25.1388888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="10.4259259259259" customWidth="1"/>
+    <col min="3" max="3" width="14.287037037037" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://www.benadryl.com/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting all other files
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/HeaderTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/HeaderTestData.xlsx
@@ -8,13 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="headerMainMenu" sheetId="1" r:id="rId1"/>
+    <sheet name="headerSubMenu" sheetId="2" r:id="rId2"/>
+    <sheet name="whereToBuy" sheetId="3" r:id="rId3"/>
+    <sheet name="language" sheetId="4" r:id="rId4"/>
+    <sheet name="search" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>testcase</t>
   </si>
@@ -31,13 +35,232 @@
     <t>Verify user is redirected to correct url after clicking on 'PRODUCTS' in the main horizontal menu</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>Products</t>
   </si>
   <si>
     <t>products</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Benadryl Difference' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Benadryl Difference</t>
+  </si>
+  <si>
+    <t>benadryl-difference</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Dosing Guide' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Dosing Guide</t>
+  </si>
+  <si>
+    <t>benadryl-dosing-guide</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Savings' in the main horizontal menu</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>save-on-benadryl</t>
+  </si>
+  <si>
+    <t>subMenu</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Adult under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>products/adult-oral</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Kid's under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <t>Kid's</t>
+  </si>
+  <si>
+    <t>products/kids</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Topical under 'PRODUCTS' menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Topical</t>
+    </r>
+  </si>
+  <si>
+    <t>products/adult-topical</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>All Products</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on Compare Benadryl under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Compare Benadryl</t>
+  </si>
+  <si>
+    <t>benadryl-difference/compare-allergy-relief-products</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Benadryl Uses" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Benadryl Difference</t>
+    </r>
+  </si>
+  <si>
+    <t>Benadryl Uses</t>
+  </si>
+  <si>
+    <t>benadryl-difference/uses-indications</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Our Ingredients" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Our Ingredients</t>
+  </si>
+  <si>
+    <t>benadryl-difference/ingredients-transparency</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "FAQ" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>faq</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Safety Information' under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>Safety Information</t>
+  </si>
+  <si>
+    <t>safety</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "About Diphenhydramine" under 'Benadryl Difference' menu</t>
+  </si>
+  <si>
+    <t>About Diphenhydramine</t>
+  </si>
+  <si>
+    <t>benadryl-difference/diphenhydramine-active-ingredient</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on "Allergies" under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Allergy &amp; Cold Guide</t>
+  </si>
+  <si>
+    <t>Allergies</t>
+  </si>
+  <si>
+    <t>allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Kid's Allergies' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Kid's Allergies</t>
+  </si>
+  <si>
+    <t>childrens-allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Itchy Skin' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Itchy Skin</t>
+  </si>
+  <si>
+    <t>itchy-skin</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Cold or Allergies?' under 'Allergy &amp; Cold Guide' menu</t>
+  </si>
+  <si>
+    <t>Cold or Allergies?</t>
+  </si>
+  <si>
+    <t>cold/cold-or-allergies</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to correct url after clicking on 'Where to buy' in the header</t>
+  </si>
+  <si>
+    <t>where-to-buy</t>
+  </si>
+  <si>
+    <t>locale</t>
+  </si>
+  <si>
+    <t>Check that user can change the locale to 'Espanol'</t>
+  </si>
+  <si>
+    <t>Espanol</t>
+  </si>
+  <si>
+    <t>https://es.benadryl.com/</t>
+  </si>
+  <si>
+    <t>Check that user can change the locale to 'English'</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>https://www.benadryl.com/</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>Verify search functionality</t>
+  </si>
+  <si>
+    <t>Benadryl</t>
+  </si>
+  <si>
+    <t>search/site/Benadryl</t>
   </si>
 </sst>
 </file>
@@ -50,8 +273,16 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,6 +296,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -521,141 +758,151 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,13 +1222,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="95.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="20.7777777777778" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -998,21 +1249,490 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="106.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="21.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="25.1388888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="10.4259259259259" customWidth="1"/>
+    <col min="3" max="3" width="14.287037037037" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://www.benadryl.com/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>